<commit_message>
Nueva librería de gráficos
</commit_message>
<xml_diff>
--- a/grafico.xlsx
+++ b/grafico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DiagnosticoPastoralConJovenesForm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianpisabarrogarcia/.bitnami/stackman/machines/xampp/volumes/root/htdocs/DiagnosticoPastoralConJovenesForm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C548394B-DC85-4A99-B3BA-0B1ED0A17821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AC513C-F95E-1943-98FE-CB4AE74615B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8465B8E-F302-4258-927F-0ADF7F2BFD60}"/>
+    <workbookView xWindow="720" yWindow="2400" windowWidth="29040" windowHeight="15840" xr2:uid="{E8465B8E-F302-4258-927F-0ADF7F2BFD60}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -837,17 +837,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5754B56F-9F80-42FD-914C-0A74840349F5}">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +858,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -890,7 +890,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -928,7 +928,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -954,7 +954,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -986,7 +986,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
         <v>120</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
         <v>121</v>
       </c>
@@ -1482,12 +1482,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C42" s="2" t="s">
         <v>123</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
         <v>124</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
         <v>125</v>
       </c>
@@ -1511,12 +1511,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C45" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
         <v>127</v>
       </c>
@@ -1524,12 +1524,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C47" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
         <v>129</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
         <v>130</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C50" s="2" t="s">
         <v>131</v>
       </c>
@@ -1553,12 +1553,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C51" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
         <v>133</v>
       </c>
@@ -1566,12 +1566,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C53" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C54" s="2" t="s">
         <v>135</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
         <v>136</v>
       </c>
@@ -1587,12 +1587,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C56" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C57" s="2" t="s">
         <v>138</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C58" s="2" t="s">
         <v>139</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C59" s="2" t="s">
         <v>140</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C60" s="2" t="s">
         <v>141</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D62" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Nueva librería de gráficos"
This reverts commit 1c2571bb3d846c7dc67a811fed3d52b8a4bf07cf.
</commit_message>
<xml_diff>
--- a/grafico.xlsx
+++ b/grafico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianpisabarrogarcia/.bitnami/stackman/machines/xampp/volumes/root/htdocs/DiagnosticoPastoralConJovenesForm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DiagnosticoPastoralConJovenesForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AC513C-F95E-1943-98FE-CB4AE74615B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C548394B-DC85-4A99-B3BA-0B1ED0A17821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="2400" windowWidth="29040" windowHeight="15840" xr2:uid="{E8465B8E-F302-4258-927F-0ADF7F2BFD60}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8465B8E-F302-4258-927F-0ADF7F2BFD60}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -837,17 +837,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5754B56F-9F80-42FD-914C-0A74840349F5}">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +858,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -890,7 +890,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -928,7 +928,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -954,7 +954,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -986,7 +986,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C39" s="2" t="s">
         <v>120</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C40" s="2" t="s">
         <v>121</v>
       </c>
@@ -1482,12 +1482,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
         <v>123</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
         <v>124</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C44" s="2" t="s">
         <v>125</v>
       </c>
@@ -1511,12 +1511,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
         <v>127</v>
       </c>
@@ -1524,12 +1524,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
         <v>129</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="2" t="s">
         <v>130</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
         <v>131</v>
       </c>
@@ -1553,12 +1553,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" s="2" t="s">
         <v>133</v>
       </c>
@@ -1566,12 +1566,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
         <v>135</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" s="2" t="s">
         <v>136</v>
       </c>
@@ -1587,12 +1587,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>138</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="2" t="s">
         <v>139</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C59" s="2" t="s">
         <v>140</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C60" s="2" t="s">
         <v>141</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D62" s="3"/>
     </row>
   </sheetData>

</xml_diff>